<commit_message>
CMD Table, 2 Mesh Models, 1 sensor, Persist_storage, LPN working
</commit_message>
<xml_diff>
--- a/Questions/Command Table Tanmay Chaturvedi.xlsx
+++ b/Questions/Command Table Tanmay Chaturvedi.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanma\SimplicityStudio\v4_workspace\course-project-TanmayChaturvedi1\Questions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2DC407-0507-4637-A071-DDAC0D66ACF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -82,39 +91,6 @@
     <t>provisioned &amp;&amp; DeviceUsesClientModel()</t>
   </si>
   <si>
-    <t>gecko_cmd_mesh_generic_client_init</t>
-  </si>
-  <si>
-    <t>Initialize the client model</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceUsesServerModel()</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_generic_server_init</t>
-  </si>
-  <si>
-    <t>Initialize the server model</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceIsOnOffPublisher()</t>
-  </si>
-  <si>
-    <t>mesh_lib_init(malloc,free,8)</t>
-  </si>
-  <si>
-    <t>Initialize the mesh library with support of up to 8 models</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceIsOnOffSubscriber()</t>
-  </si>
-  <si>
-    <t>mesh_lib_init(malloc,free,9), mesh_lib_generic_server_register_handler, mesh_lib_generic_server_update, mesh_lib_generic_server_publish</t>
-  </si>
-  <si>
-    <t>See init_models, onoff_request, onoff_update_and_publish in lightbulb.c, soc-btmesh-light example</t>
-  </si>
-  <si>
     <t>!provisioned</t>
   </si>
   <si>
@@ -145,21 +121,9 @@
     <t>"Provision Fail"</t>
   </si>
   <si>
-    <t>provisioned</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_lpn_init; gecko_cmd_mesh_lpn_configure; gecko_cmd_mesh_lpn_establish_friendship</t>
-  </si>
-  <si>
     <t>gecko_evt_mesh_lpn_friendship_established_id, gecko_evt_mesh_lpn_friendship_failed_id, gecko_evt_mesh_lpn_friendship_terminated_id</t>
   </si>
   <si>
-    <t>"LPN Init done"</t>
-  </si>
-  <si>
-    <t>When Provisioned, Press reset buttong and after initialization, lpn_init() function is called which has lpn and friendship init commands</t>
-  </si>
-  <si>
     <t>gecko_evt_mesh_lpn_friendship_established_id</t>
   </si>
   <si>
@@ -184,18 +148,6 @@
     <t>When friendship is terminated, retry after 2 seconds to find a friend and establish friendship</t>
   </si>
   <si>
-    <t>gecko_evt_mesh_generic_server_client_request_id</t>
-  </si>
-  <si>
-    <t>DeviceUsesServerModel()</t>
-  </si>
-  <si>
-    <t>mesh_lib_generic_server_event_handler</t>
-  </si>
-  <si>
-    <t>gecko_evt_mesh_generic_server_state_changed_id</t>
-  </si>
-  <si>
     <t>gecko_evt_le_connection_opened_id</t>
   </si>
   <si>
@@ -214,72 +166,111 @@
     <t>Factory reset when requested by provisioner, using the same 2 second soft timer delay</t>
   </si>
   <si>
-    <t>gecko_evt_system_external_signal_id</t>
-  </si>
-  <si>
-    <t>Handle scheduler events</t>
-  </si>
-  <si>
-    <t>Button 0 press or release event &amp;&amp; DeviceIsOnOffPublisher()</t>
-  </si>
-  <si>
     <t>mesh_lib_generic_client_publish</t>
   </si>
   <si>
-    <t>Publish button press or release using the on off model.  Press = on</t>
-  </si>
-  <si>
-    <t>client request or server change callback for generic on/off model</t>
-  </si>
-  <si>
-    <t>"Button Pressed" or "Button Released"</t>
-  </si>
-  <si>
-    <t>Display the state of the button on the subscriber</t>
+    <t>gecko_cmd_mesh_generic_client_init, mesh_lib_init(malloc,free,8), gecko_cmd_mesh_lpn_init; gecko_cmd_mesh_lpn_configure; gecko_cmd_mesh_lpn_establish_friendship</t>
+  </si>
+  <si>
+    <t>"LPN Init Done"</t>
+  </si>
+  <si>
+    <t>Initialize the client model and mesh library with support of up to 8 models and start looking for friend. When Provisioned, Press reset button and after initialization, lpn_init() function is called which has lpn and friendship init commands</t>
+  </si>
+  <si>
+    <t>gecko_cmd_hardware_set_soft_timer(LUX DATA timer handler)</t>
+  </si>
+  <si>
+    <t>LUX Data timer handle</t>
+  </si>
+  <si>
+    <t>"ABOVE THRESHOLD" / "BELOW THRESHOLD"</t>
+  </si>
+  <si>
+    <t>"Lux = XXX.YY" on DISPLAY_ROW_TEMPVALUE</t>
+  </si>
+  <si>
+    <t>Publishes Lux data and On/Off if the lux value greater/less than preset threshold to the friend node</t>
+  </si>
+  <si>
+    <t>gecko_evt_gatt_server_user_write_request_id</t>
+  </si>
+  <si>
+    <t>gecko_cmd_gatt_server_send_user_write_response, gecko_cmd_le_connection_close</t>
+  </si>
+  <si>
+    <t>For firmware updates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If no friend </t>
+  </si>
+  <si>
+    <t>Keep finding friend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="10.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -287,7 +278,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -297,75 +288,374 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.0"/>
-    <col customWidth="1" min="2" max="2" width="24.71"/>
-    <col customWidth="1" min="3" max="3" width="22.57"/>
-    <col customWidth="1" min="4" max="4" width="21.57"/>
-    <col customWidth="1" min="5" max="5" width="20.14"/>
-    <col customWidth="1" min="6" max="6" width="22.0"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +697,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -428,7 +718,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -447,8 +737,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -466,355 +756,292 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>25</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>27</v>
+      <c r="E6" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>39</v>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>41</v>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4" t="s">
+    <row r="14" spans="1:26" s="14" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6" t="s">
+    <row r="17" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="6" t="s">
+    </row>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>51</v>
-      </c>
+    <row r="19" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>51</v>
-      </c>
+    <row r="20" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="9" t="s">
-        <v>56</v>
-      </c>
+    <row r="21" spans="1:7" ht="14.25" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1784,13 +2011,8 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
-    <row r="1003" ht="14.25" customHeight="1"/>
-    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>